<commit_message>
refactor and create sprint review powerpoint
</commit_message>
<xml_diff>
--- a/docs/Project Gantt Chart.xlsx
+++ b/docs/Project Gantt Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b74ff9ac3a48cbb/UWE/Year 3/Enterprise Systems Development/Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Projects\Enterprise-Systems-Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="8_{FFDF537C-00C2-4742-B60C-89BC8BE859CF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{89549BA0-2EBE-4942-9794-0D5A9537B00F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B96E1E-0A0E-4352-B583-AC672672D69C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{F511A3B4-8B61-4D68-A2C0-45021F7B5F45}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" xr2:uid="{F511A3B4-8B61-4D68-A2C0-45021F7B5F45}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -138,7 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +173,12 @@
       <b/>
       <sz val="22"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -281,73 +287,76 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -666,395 +675,403 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D53BBCF-509D-459A-91AD-8D778710031E}">
   <dimension ref="B1:M20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="64" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="7" width="30.7109375" customWidth="1"/>
-    <col min="8" max="13" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
+    <col min="3" max="7" width="30.7265625" customWidth="1"/>
+    <col min="8" max="13" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" s="4" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="3" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    <row r="1" spans="2:13" s="3" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+    </row>
+    <row r="3" spans="2:13" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2">
-        <v>2</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="10"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="F4" s="20"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2">
-        <v>2</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="10"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+      <c r="F5" s="20"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2">
-        <v>2</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="2">
-        <v>2</v>
-      </c>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="H7" s="3" t="s">
+      <c r="F7" s="20"/>
+      <c r="H7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2">
-        <v>2</v>
-      </c>
-      <c r="E8" s="10" t="s">
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="2" t="s">
+      <c r="F8" s="20"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="2">
-        <v>2</v>
-      </c>
-      <c r="E9" s="10" t="s">
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="2" t="s">
+      <c r="F9" s="20"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="2">
-        <v>2</v>
-      </c>
-      <c r="E10" s="10" t="s">
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-    </row>
-    <row r="12" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H12" s="6" t="s">
+      <c r="F10" s="20"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="2:13" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H12" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+    </row>
+    <row r="13" spans="2:13" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="5">
-        <v>1</v>
-      </c>
-      <c r="I13" s="5">
-        <v>2</v>
-      </c>
-      <c r="J13" s="5">
+      <c r="H13" s="4">
+        <v>1</v>
+      </c>
+      <c r="I13" s="4">
+        <v>2</v>
+      </c>
+      <c r="J13" s="4">
         <v>3</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="4">
         <v>4</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="4">
         <v>5</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="12">
-        <v>1</v>
-      </c>
-      <c r="D14" s="12">
-        <v>2</v>
-      </c>
-      <c r="E14" s="12">
-        <v>1</v>
-      </c>
-      <c r="F14" s="12">
-        <v>1</v>
-      </c>
-      <c r="G14" s="11">
-        <v>1</v>
-      </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="23"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9">
+        <v>2</v>
+      </c>
+      <c r="E14" s="9">
+        <v>1</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1</v>
+      </c>
+      <c r="H14" s="17"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="19"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="13">
-        <v>1</v>
-      </c>
-      <c r="D15" s="13">
-        <v>2</v>
-      </c>
-      <c r="E15" s="13">
-        <v>1</v>
-      </c>
-      <c r="F15" s="13">
-        <v>1</v>
-      </c>
-      <c r="G15" s="11">
-        <v>1</v>
-      </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="23"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
+      <c r="C15" s="10">
+        <v>1</v>
+      </c>
+      <c r="D15" s="10">
+        <v>2</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1</v>
+      </c>
+      <c r="G15" s="8">
+        <v>1</v>
+      </c>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="19"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="13">
-        <v>1</v>
-      </c>
-      <c r="D16" s="13">
-        <v>2</v>
-      </c>
-      <c r="E16" s="13">
-        <v>1</v>
-      </c>
-      <c r="F16" s="13">
-        <v>1</v>
-      </c>
-      <c r="G16" s="11">
-        <v>1</v>
-      </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="23"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
+      <c r="C16" s="10">
+        <v>1</v>
+      </c>
+      <c r="D16" s="10">
+        <v>2</v>
+      </c>
+      <c r="E16" s="10">
+        <v>1</v>
+      </c>
+      <c r="F16" s="10">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8">
+        <v>1</v>
+      </c>
+      <c r="H16" s="17"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="19"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="13">
-        <v>1</v>
-      </c>
-      <c r="D17" s="13">
-        <v>2</v>
-      </c>
-      <c r="E17" s="13">
-        <v>1</v>
-      </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="11">
-        <v>0</v>
-      </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="23"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
+      <c r="C17" s="10">
+        <v>1</v>
+      </c>
+      <c r="D17" s="10">
+        <v>2</v>
+      </c>
+      <c r="E17" s="10">
+        <v>1</v>
+      </c>
+      <c r="F17" s="10">
+        <v>2</v>
+      </c>
+      <c r="G17" s="8">
+        <v>1</v>
+      </c>
+      <c r="H17" s="23"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="19"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="13">
-        <v>1</v>
-      </c>
-      <c r="D18" s="13">
-        <v>2</v>
-      </c>
-      <c r="E18" s="13">
-        <v>1</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="11">
-        <v>0</v>
-      </c>
-      <c r="H18" s="22"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="23"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
+      <c r="C18" s="10">
+        <v>1</v>
+      </c>
+      <c r="D18" s="10">
+        <v>2</v>
+      </c>
+      <c r="E18" s="10">
+        <v>1</v>
+      </c>
+      <c r="F18" s="10">
+        <v>2</v>
+      </c>
+      <c r="G18" s="8">
+        <v>1</v>
+      </c>
+      <c r="H18" s="23"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="19"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="13">
-        <v>1</v>
-      </c>
-      <c r="D19" s="13">
-        <v>2</v>
-      </c>
-      <c r="E19" s="13">
-        <v>1</v>
-      </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="11">
-        <v>0</v>
-      </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="23"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
+      <c r="C19" s="10">
+        <v>1</v>
+      </c>
+      <c r="D19" s="10">
+        <v>2</v>
+      </c>
+      <c r="E19" s="10">
+        <v>1</v>
+      </c>
+      <c r="F19" s="10">
+        <v>2</v>
+      </c>
+      <c r="G19" s="8">
+        <v>1</v>
+      </c>
+      <c r="H19" s="23"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="19"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="13">
-        <v>1</v>
-      </c>
-      <c r="D20" s="13">
-        <v>2</v>
-      </c>
-      <c r="E20" s="13">
-        <v>1</v>
-      </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="11">
-        <v>0</v>
-      </c>
-      <c r="H20" s="22"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="23"/>
+      <c r="C20" s="10">
+        <v>1</v>
+      </c>
+      <c r="D20" s="10">
+        <v>2</v>
+      </c>
+      <c r="E20" s="10">
+        <v>1</v>
+      </c>
+      <c r="F20" s="10">
+        <v>2</v>
+      </c>
+      <c r="G20" s="8">
+        <v>1</v>
+      </c>
+      <c r="H20" s="23"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>